<commit_message>
fix for each loop
</commit_message>
<xml_diff>
--- a/InAuto_Project_2200589F_2202465G/InternshipLinks.xlsx
+++ b/InAuto_Project_2200589F_2202465G/InternshipLinks.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/78df99500250e0aa/Documents/GitHub/InAuto/InAuto_Project_2200589F_2202465G/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="192" documentId="11_2CD8505CD931ACBCCD46FCF201C52297C3D0BD78" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{AA65D27C-27B2-4B12-9765-BEF278BD348B}"/>
+  <xr:revisionPtr revIDLastSave="270" documentId="11_2CD8505CD931ACBCCD46FCF201C52297C3D0BD78" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{5897ABC4-C0C4-4F2A-B34C-90E428A35B9C}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="4872" yWindow="3360" windowWidth="17280" windowHeight="8880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="2" r:id="rId1"/>
@@ -34,15 +34,39 @@
     <t>Url</t>
   </si>
   <si>
+    <t>SATS Ltd</t>
+  </si>
+  <si>
+    <t>Internship</t>
+  </si>
+  <si>
+    <t>Less than a year</t>
+  </si>
+  <si>
+    <t>https://glints.com/sg/opportunities/jobs/operational-excellence-intern/a8b2710b-5c6d-4e97-b1cd-13d0b32e5806?utm_referrer=explore</t>
+  </si>
+  <si>
+    <t>https://glints.com/sg/opportunities/jobs/airport-lounge-bartender-intern-6-months/a343d364-5c0e-4c45-a644-1d5b1246e87e?utm_referrer=explore</t>
+  </si>
+  <si>
+    <t>https://glints.com/sg/opportunities/jobs/airport-transit-lounge-intern-6-months/bf8c233d-3e33-4cfa-84cc-c9f709636531?utm_referrer=explore</t>
+  </si>
+  <si>
+    <t>https://glints.com/sg/opportunities/jobs/robotic-process-automation-rpa-and-power-platform-intern-6-mth/a6b35435-4061-4a99-adef-27384f1d1be8?utm_referrer=explore</t>
+  </si>
+  <si>
+    <t>https://glints.com/sg/opportunities/jobs/talent-acquisition-intern-jan-jun-2024/280b0ed4-eb40-44a1-80bf-19adbeb474b5?utm_referrer=explore</t>
+  </si>
+  <si>
+    <t>1st Choice Recruit Pte Ltd</t>
+  </si>
+  <si>
     <t>Full-Time</t>
   </si>
   <si>
     <t>1 – 3 years</t>
   </si>
   <si>
-    <t>1st Choice Recruit Pte Ltd</t>
-  </si>
-  <si>
     <t>https://glints.com/sg/opportunities/jobs/import-executive/c1b89a38-2ce8-42b4-a828-c88cb87909d4?utm_referrer=explore</t>
   </si>
   <si>
@@ -50,47 +74,16 @@
   </si>
   <si>
     <t>https://glints.com/sg/opportunities/jobs/fun-sales-assistant-retail/a04bbd98-f889-47b8-aa4a-7e5158a30933?utm_referrer=explore</t>
-  </si>
-  <si>
-    <t>SATS Ltd</t>
-  </si>
-  <si>
-    <t>Internship</t>
-  </si>
-  <si>
-    <t>Less than a year</t>
-  </si>
-  <si>
-    <t>https://glints.com/sg/opportunities/jobs/airport-transit-lounge-intern-6-months/bf8c233d-3e33-4cfa-84cc-c9f709636531?utm_referrer=explore</t>
-  </si>
-  <si>
-    <t>https://glints.com/sg/opportunities/jobs/airport-lounge-bartender-intern-6-months/a343d364-5c0e-4c45-a644-1d5b1246e87e?utm_referrer=explore</t>
-  </si>
-  <si>
-    <t>https://glints.com/sg/opportunities/jobs/operational-excellence-intern/a8b2710b-5c6d-4e97-b1cd-13d0b32e5806?utm_referrer=explore</t>
-  </si>
-  <si>
-    <t>https://glints.com/sg/opportunities/jobs/talent-acquisition-intern-jan-jun-2024/280b0ed4-eb40-44a1-80bf-19adbeb474b5?utm_referrer=explore</t>
-  </si>
-  <si>
-    <t>https://glints.com/sg/opportunities/jobs/robotic-process-automation-rpa-and-power-platform-intern-6-mth/a6b35435-4061-4a99-adef-27384f1d1be8?utm_referrer=explore</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
     </font>
@@ -112,16 +105,13 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyBorder="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1" applyProtection="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFill="1" applyAlignment="1" applyProtection="1"/>
   </cellXfs>
-  <cellStyles count="2">
-    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
+  <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -425,7 +415,7 @@
   <dimension ref="A1:D8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -453,100 +443,100 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>6</v>
+        <v>12</v>
       </c>
       <c r="B2" t="s">
-        <v>4</v>
+        <v>13</v>
       </c>
       <c r="C2" t="s">
-        <v>5</v>
-      </c>
-      <c r="D2" s="1" t="s">
-        <v>7</v>
+        <v>14</v>
+      </c>
+      <c r="D2" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>8</v>
+        <v>16</v>
       </c>
       <c r="B3" t="s">
-        <v>4</v>
+        <v>13</v>
       </c>
       <c r="C3" t="s">
-        <v>5</v>
+        <v>14</v>
       </c>
       <c r="D3" t="s">
-        <v>9</v>
+        <v>17</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>10</v>
+        <v>4</v>
       </c>
       <c r="B4" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="C4" t="s">
-        <v>12</v>
+        <v>6</v>
       </c>
       <c r="D4" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>10</v>
+        <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="C5" t="s">
-        <v>12</v>
+        <v>6</v>
       </c>
       <c r="D5" t="s">
-        <v>14</v>
+        <v>8</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>10</v>
+        <v>4</v>
       </c>
       <c r="B6" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="C6" t="s">
-        <v>12</v>
+        <v>6</v>
       </c>
       <c r="D6" t="s">
-        <v>15</v>
+        <v>7</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>10</v>
+        <v>4</v>
       </c>
       <c r="B7" t="s">
+        <v>5</v>
+      </c>
+      <c r="C7" t="s">
+        <v>6</v>
+      </c>
+      <c r="D7" t="s">
         <v>11</v>
-      </c>
-      <c r="C7" t="s">
-        <v>12</v>
-      </c>
-      <c r="D7" t="s">
-        <v>16</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
+        <v>4</v>
+      </c>
+      <c r="B8" t="s">
+        <v>5</v>
+      </c>
+      <c r="C8" t="s">
+        <v>6</v>
+      </c>
+      <c r="D8" t="s">
         <v>10</v>
-      </c>
-      <c r="B8" t="s">
-        <v>11</v>
-      </c>
-      <c r="C8" t="s">
-        <v>12</v>
-      </c>
-      <c r="D8" t="s">
-        <v>17</v>
       </c>
     </row>
   </sheetData>
@@ -555,9 +545,6 @@
     <sortCondition ref="B1"/>
     <sortCondition ref="C1"/>
   </sortState>
-  <hyperlinks>
-    <hyperlink ref="D2" r:id="rId1" xr:uid="{29213148-9313-48F3-8074-194DDDBCA059}"/>
-  </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="0.75" bottom="0.5" header="0.5" footer="0.75"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
fixed the click in first part
</commit_message>
<xml_diff>
--- a/InAuto_Project_2200589F_2202465G/InternshipLinks.xlsx
+++ b/InAuto_Project_2200589F_2202465G/InternshipLinks.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/78df99500250e0aa/Documents/GitHub/InAuto/InAuto_Project_2200589F_2202465G/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="70" documentId="13_ncr:1_{ED0C76FE-FE4C-42B2-AA37-CC2E5182DCC6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{1BBBA482-0C00-44C8-B613-AD8CEC8A599F}"/>
+  <xr:revisionPtr revIDLastSave="83" documentId="13_ncr:1_{ED0C76FE-FE4C-42B2-AA37-CC2E5182DCC6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{16E32093-ECF4-4E08-9C51-FCD5CBD6DAF0}"/>
   <bookViews>
     <workbookView xWindow="5220" yWindow="3360" windowWidth="17280" windowHeight="8880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="124" uniqueCount="69">
   <si>
     <t>Company</t>
   </si>
@@ -112,19 +112,121 @@
     <t>https://glints.com/sg/opportunities/jobs/singapore-software-engineer-fresh-grad-also-welcome/5f2526b9-7d5f-4ae2-b1b9-0be2274bd696?utm_referrer=explore</t>
   </si>
   <si>
-    <t>Mgg Software Pte Ltd</t>
-  </si>
-  <si>
-    <t>https://glints.com/sg/opportunities/jobs/intern-bids-and-proposal/4f83d138-dae5-4a84-9ba1-9350933b8203?utm_referrer=explore</t>
-  </si>
-  <si>
     <t>System Technic Engineering Pte Ltd</t>
   </si>
   <si>
     <t>https://glints.com/sg/opportunities/jobs/engineering-intern/d1f645f0-696d-4682-bc47-1a174108c33a?utm_referrer=explore</t>
   </si>
   <si>
-    <t>https://glints.com/sg/opportunities/jobs/administration-assistant/515c46cf-61dd-424e-8733-029faa22556d?utm_referrer=explore</t>
+    <t>Atomionics</t>
+  </si>
+  <si>
+    <t>Software Testing</t>
+  </si>
+  <si>
+    <t>https://glints.com/sg/opportunities/jobs/software-engineering-intern-for-quantum-sensor-immediate/12e16672-150f-4319-8945-0e089ff0dfb2?utm_referrer=explore</t>
+  </si>
+  <si>
+    <t>5 – 10 years</t>
+  </si>
+  <si>
+    <t>https://glints.com/sg/opportunities/jobs/software-developer/3d2bc63c-42e4-4abe-b581-7e77712ef51b?utm_referrer=explore</t>
+  </si>
+  <si>
+    <t>Machine Learning</t>
+  </si>
+  <si>
+    <t>https://glints.com/sg/opportunities/jobs/software-engineering-python-intern-jan-2024-or-later/4591a978-859f-489e-9136-dcbe755d797c?utm_referrer=explore</t>
+  </si>
+  <si>
+    <t>MATLAB</t>
+  </si>
+  <si>
+    <t>https://glints.com/sg/opportunities/jobs/software-controls-engineering-intern-jan-2024-or-later/f0b28d2f-610d-4641-b533-cb75f329f05a?utm_referrer=explore</t>
+  </si>
+  <si>
+    <t>Hypotenuse AI</t>
+  </si>
+  <si>
+    <t>3 – 5 years</t>
+  </si>
+  <si>
+    <t>https://glints.com/sg/opportunities/jobs/senior-software-engineer/8ebfc23d-78f6-4adb-97d7-8917e36cb11f?utm_referrer=explore</t>
+  </si>
+  <si>
+    <t>https://glints.com/sg/opportunities/jobs/senior-software-developer/bb603918-ab34-4892-89bc-017d3ed47bb7?utm_referrer=explore</t>
+  </si>
+  <si>
+    <t>The Swim Starter</t>
+  </si>
+  <si>
+    <t>https://glints.com/sg/opportunities/jobs/senior-software-engineer/983103cd-eb96-44ea-b801-4a18038e285b?utm_referrer=explore</t>
+  </si>
+  <si>
+    <t>One North Consulting Pte Ltd</t>
+  </si>
+  <si>
+    <t>https://glints.com/sg/opportunities/jobs/senior-manual-software-tester/23eb27e8-94cc-435a-ad27-8fb713f59881?utm_referrer=explore</t>
+  </si>
+  <si>
+    <t>Aztech Technologies Pte Ltd</t>
+  </si>
+  <si>
+    <t>MySQL</t>
+  </si>
+  <si>
+    <t>https://glints.com/sg/opportunities/jobs/r-and-d-software-internship/8da1f5d8-f341-4eae-9be8-f899b3530174?utm_referrer=explore</t>
+  </si>
+  <si>
+    <t>Transcelestial Technologies</t>
+  </si>
+  <si>
+    <t>https://glints.com/sg/opportunities/jobs/senior-manufacturing-software-engineer/0b12c9e4-896a-4f4f-9b99-b9ded5ab0212?utm_referrer=explore</t>
+  </si>
+  <si>
+    <t>Problem Solving Skills</t>
+  </si>
+  <si>
+    <t>https://glints.com/sg/opportunities/jobs/r-and-d-mechanical-engineering-internship/a6dc8700-63b7-49bc-930f-9683b8a3c0d1?utm_referrer=explore</t>
+  </si>
+  <si>
+    <t>Noak</t>
+  </si>
+  <si>
+    <t>iOS Development</t>
+  </si>
+  <si>
+    <t>https://glints.com/sg/opportunities/jobs/software-qa-engineer-includes-equity/7c4c3307-ae1e-45b6-96b1-3b72dfb5f651?utm_referrer=explore</t>
+  </si>
+  <si>
+    <t>Software Engineering</t>
+  </si>
+  <si>
+    <t>https://glints.com/sg/opportunities/jobs/full-stack-software-engineer-intern-6-months/e6728566-e76f-4972-8705-f73e9ceff3d7?utm_referrer=explore</t>
+  </si>
+  <si>
+    <t>Contract</t>
+  </si>
+  <si>
+    <t>https://glints.com/sg/opportunities/jobs/remote-software-engineer-for-quantum-sensor-immediate/9d90f867-1ffe-4c83-a3ab-24354745c197?utm_referrer=explore</t>
+  </si>
+  <si>
+    <t>Aha AI</t>
+  </si>
+  <si>
+    <t>https://glints.com/sg/opportunities/jobs/singapore-senior-engineering-lead-full-remote/54891082-34ec-4471-90b9-218c91d8709a?utm_referrer=explore</t>
+  </si>
+  <si>
+    <t>Circuit Design</t>
+  </si>
+  <si>
+    <t>https://glints.com/sg/opportunities/jobs/electronics-engineering-intern-jan-2024-or-later/8d80ea0a-8f51-4ef3-988c-e6d75c9551b1?utm_referrer=explore</t>
+  </si>
+  <si>
+    <t>Verilog</t>
+  </si>
+  <si>
+    <t>https://glints.com/sg/opportunities/jobs/firmware-engineering-intern-jan-2024-or-later/b8bd3a3c-b0b4-4d84-af24-ad2dac43e155?utm_referrer=explore</t>
   </si>
 </sst>
 </file>
@@ -463,7 +565,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D16"/>
+  <dimension ref="A1:D31"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="D2" sqref="D2"/>
@@ -473,8 +575,8 @@
   <cols>
     <col min="1" max="1" width="29.88671875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="9.109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="14.109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="136.44140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="18.44140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="139.77734375" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="140.109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -508,175 +610,175 @@
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>24</v>
+        <v>63</v>
       </c>
       <c r="B3" t="s">
         <v>5</v>
       </c>
       <c r="C3" t="s">
-        <v>22</v>
+        <v>35</v>
       </c>
       <c r="D3" t="s">
-        <v>25</v>
+        <v>64</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>26</v>
+        <v>32</v>
       </c>
       <c r="B4" t="s">
-        <v>5</v>
+        <v>61</v>
       </c>
       <c r="C4" t="s">
-        <v>22</v>
+        <v>42</v>
       </c>
       <c r="D4" t="s">
-        <v>27</v>
+        <v>62</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="B5" t="s">
         <v>4</v>
       </c>
       <c r="C5" t="s">
-        <v>22</v>
+        <v>65</v>
       </c>
       <c r="D5" t="s">
-        <v>31</v>
+        <v>66</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>21</v>
+        <v>32</v>
       </c>
       <c r="B6" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C6" t="s">
-        <v>22</v>
+        <v>37</v>
       </c>
       <c r="D6" t="s">
-        <v>23</v>
+        <v>38</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>9</v>
+        <v>32</v>
       </c>
       <c r="B7" t="s">
         <v>4</v>
       </c>
       <c r="C7" t="s">
-        <v>6</v>
+        <v>39</v>
       </c>
       <c r="D7" t="s">
-        <v>10</v>
+        <v>40</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>9</v>
+        <v>32</v>
       </c>
       <c r="B8" t="s">
         <v>4</v>
       </c>
       <c r="C8" t="s">
-        <v>6</v>
+        <v>33</v>
       </c>
       <c r="D8" t="s">
-        <v>15</v>
+        <v>34</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>11</v>
+        <v>32</v>
       </c>
       <c r="B9" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C9" t="s">
-        <v>6</v>
+        <v>67</v>
       </c>
       <c r="D9" t="s">
-        <v>20</v>
+        <v>68</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>11</v>
+        <v>49</v>
       </c>
       <c r="B10" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C10" t="s">
-        <v>6</v>
+        <v>50</v>
       </c>
       <c r="D10" t="s">
-        <v>12</v>
+        <v>51</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>18</v>
+        <v>49</v>
       </c>
       <c r="B11" t="s">
         <v>4</v>
       </c>
       <c r="C11" t="s">
-        <v>6</v>
+        <v>54</v>
       </c>
       <c r="D11" t="s">
-        <v>19</v>
+        <v>55</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>7</v>
+        <v>41</v>
       </c>
       <c r="B12" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C12" t="s">
-        <v>6</v>
+        <v>42</v>
       </c>
       <c r="D12" t="s">
-        <v>8</v>
+        <v>43</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>32</v>
+        <v>41</v>
       </c>
       <c r="B13" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C13" t="s">
-        <v>22</v>
+        <v>59</v>
       </c>
       <c r="D13" t="s">
-        <v>34</v>
+        <v>60</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>32</v>
+        <v>24</v>
       </c>
       <c r="B14" t="s">
         <v>5</v>
       </c>
       <c r="C14" t="s">
-        <v>6</v>
+        <v>22</v>
       </c>
       <c r="D14" t="s">
-        <v>33</v>
+        <v>25</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="B15" t="s">
         <v>5</v>
@@ -685,25 +787,235 @@
         <v>22</v>
       </c>
       <c r="D15" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
+        <v>26</v>
+      </c>
+      <c r="B16" t="s">
+        <v>5</v>
+      </c>
+      <c r="C16" t="s">
+        <v>35</v>
+      </c>
+      <c r="D16" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A17" t="s">
+        <v>26</v>
+      </c>
+      <c r="B17" t="s">
+        <v>5</v>
+      </c>
+      <c r="C17" t="s">
+        <v>35</v>
+      </c>
+      <c r="D17" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A18" t="s">
+        <v>21</v>
+      </c>
+      <c r="B18" t="s">
+        <v>5</v>
+      </c>
+      <c r="C18" t="s">
+        <v>22</v>
+      </c>
+      <c r="D18" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A19" t="s">
+        <v>9</v>
+      </c>
+      <c r="B19" t="s">
+        <v>4</v>
+      </c>
+      <c r="C19" t="s">
+        <v>6</v>
+      </c>
+      <c r="D19" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A20" t="s">
+        <v>9</v>
+      </c>
+      <c r="B20" t="s">
+        <v>4</v>
+      </c>
+      <c r="C20" t="s">
+        <v>6</v>
+      </c>
+      <c r="D20" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A21" t="s">
+        <v>56</v>
+      </c>
+      <c r="B21" t="s">
+        <v>5</v>
+      </c>
+      <c r="C21" t="s">
+        <v>57</v>
+      </c>
+      <c r="D21" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A22" t="s">
+        <v>47</v>
+      </c>
+      <c r="B22" t="s">
+        <v>5</v>
+      </c>
+      <c r="C22" t="s">
+        <v>42</v>
+      </c>
+      <c r="D22" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A23" t="s">
+        <v>11</v>
+      </c>
+      <c r="B23" t="s">
+        <v>5</v>
+      </c>
+      <c r="C23" t="s">
+        <v>6</v>
+      </c>
+      <c r="D23" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A24" t="s">
+        <v>11</v>
+      </c>
+      <c r="B24" t="s">
+        <v>5</v>
+      </c>
+      <c r="C24" t="s">
+        <v>6</v>
+      </c>
+      <c r="D24" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A25" t="s">
+        <v>18</v>
+      </c>
+      <c r="B25" t="s">
+        <v>4</v>
+      </c>
+      <c r="C25" t="s">
+        <v>6</v>
+      </c>
+      <c r="D25" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A26" t="s">
+        <v>7</v>
+      </c>
+      <c r="B26" t="s">
+        <v>4</v>
+      </c>
+      <c r="C26" t="s">
+        <v>6</v>
+      </c>
+      <c r="D26" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A27" t="s">
+        <v>30</v>
+      </c>
+      <c r="B27" t="s">
+        <v>5</v>
+      </c>
+      <c r="C27" t="s">
+        <v>6</v>
+      </c>
+      <c r="D27" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A28" t="s">
+        <v>45</v>
+      </c>
+      <c r="B28" t="s">
+        <v>5</v>
+      </c>
+      <c r="C28" t="s">
+        <v>42</v>
+      </c>
+      <c r="D28" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A29" t="s">
+        <v>52</v>
+      </c>
+      <c r="B29" t="s">
+        <v>5</v>
+      </c>
+      <c r="C29" t="s">
+        <v>35</v>
+      </c>
+      <c r="D29" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A30" t="s">
+        <v>28</v>
+      </c>
+      <c r="B30" t="s">
+        <v>5</v>
+      </c>
+      <c r="C30" t="s">
+        <v>22</v>
+      </c>
+      <c r="D30" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A31" t="s">
         <v>13</v>
       </c>
-      <c r="B16" t="s">
-        <v>4</v>
-      </c>
-      <c r="C16" t="s">
+      <c r="B31" t="s">
+        <v>4</v>
+      </c>
+      <c r="C31" t="s">
         <v>6</v>
       </c>
-      <c r="D16" t="s">
+      <c r="D31" t="s">
         <v>14</v>
       </c>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:D16">
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:D31">
     <sortCondition ref="A1"/>
     <sortCondition ref="B1"/>
     <sortCondition ref="C1"/>

</xml_diff>